<commit_message>
Checklist_45 for the 45 degree movement. Checklist_Straight_Rotate works on command F100 for 100cm , F110 for 110cm. not accurate yet
L/R180 will be L/R for 180 degrees. L/R360 will be 360 degrees.

Added ticks/degree reading for some simple formulation.
</commit_message>
<xml_diff>
--- a/Arduino/Proximity Sensor Readings Final.xlsx
+++ b/Arduino/Proximity Sensor Readings Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/659c071ba0b66ebb/Documents/GitHub/MDP-Group-10/Arduino/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\MDP-Group-10\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{5644D56C-A0A3-4FCF-955F-D2339E29F552}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EECBB3D9-5B83-4A69-94A5-BC81814F1F83}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F7F647-1D91-4F77-B9C5-253BAD54F73E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{81B1DE48-6FA4-4ADC-BDBF-E46C1CA0A339}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{81B1DE48-6FA4-4ADC-BDBF-E46C1CA0A339}"/>
   </bookViews>
   <sheets>
     <sheet name="Proximity Sensor Calibration" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="32">
   <si>
     <t>1st</t>
   </si>
@@ -121,6 +121,15 @@
   <si>
     <t>Sensor A5 Long Range</t>
   </si>
+  <si>
+    <t>Rotate</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Ticks</t>
+  </si>
 </sst>
 </file>
 
@@ -182,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -205,6 +214,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B95ED87-4D0C-40C6-B81A-414C63090E9A}">
-  <dimension ref="A1:AV109"/>
+  <dimension ref="A1:AV118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="D85" workbookViewId="0">
+      <selection activeCell="O118" sqref="O118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7460,6 +7472,65 @@
         <v>133.73500000000001</v>
       </c>
     </row>
+    <row r="112" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="D112" t="s">
+        <v>29</v>
+      </c>
+      <c r="F112" t="s">
+        <v>30</v>
+      </c>
+      <c r="G112" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F113" s="9">
+        <v>87</v>
+      </c>
+      <c r="G113" s="9">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="114" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F114" s="9">
+        <v>170</v>
+      </c>
+      <c r="G114" s="9">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="115" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F115" s="9">
+        <v>255</v>
+      </c>
+      <c r="G115" s="9">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="116" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F116" s="9">
+        <v>340</v>
+      </c>
+      <c r="G116" s="9">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="117" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F117" s="9">
+        <v>680</v>
+      </c>
+      <c r="G117" s="9">
+        <v>3080</v>
+      </c>
+    </row>
+    <row r="118" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F118" s="9">
+        <v>825</v>
+      </c>
+      <c r="G118" s="9">
+        <v>3626</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A91:A92"/>

</xml_diff>